<commit_message>
Jun 11, 2024, 3:10 PM
</commit_message>
<xml_diff>
--- a/Main/static/CSVs/PC Features List.xlsx
+++ b/Main/static/CSVs/PC Features List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitProjects\CS50-FinalProject\Main\static\CSVs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2917A4D4-4C5A-403A-83C1-BD04660D6F2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DA7DEF-DF2E-4356-941E-602E40A7056C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14970" yWindow="0" windowWidth="13935" windowHeight="15585" xr2:uid="{B488902C-D55E-47C3-8D97-FFB9C3833CE3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B488902C-D55E-47C3-8D97-FFB9C3833CE3}"/>
   </bookViews>
   <sheets>
     <sheet name="pc_feature_list" sheetId="4" r:id="rId1"/>

</xml_diff>

<commit_message>
Jun 11, 2024, 3:55 PM
</commit_message>
<xml_diff>
--- a/Main/static/CSVs/PC Features List.xlsx
+++ b/Main/static/CSVs/PC Features List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitProjects\CS50-FinalProject\Main\static\CSVs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DA7DEF-DF2E-4356-941E-602E40A7056C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52153E2-E89D-4677-B484-2A6C5E86BB66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B488902C-D55E-47C3-8D97-FFB9C3833CE3}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="159">
   <si>
     <t>Fighter</t>
   </si>
@@ -111,12 +111,6 @@
     <t>When you are wielding a melee weapon in one hand and no other weapons, you gain a +2 bonus to damage rolls with that weapon.</t>
   </si>
   <si>
-    <t>When you roll a 1 or 2 on a damage die for an attack you make with a melee weapon that you are wielding with two hands, you can reroll the die and must use the new roll, even if the new roll is a 1 or a 2. The weapon must have the two-handed or versatile property for you to gain this benefit.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Starting at 2nd level Fighter, you can push yourself beyond your normal limits for a moment. On your turn, you can take one additional action on top of your regular action and a possible bonus action. Once you use this feature, you must finish a short or long rest before you can use it again. Starting at 17th level, you can use it twice before a rest, but only once on the same turn. </t>
-  </si>
-  <si>
     <t>At 3rd level Fighter, you choose an archetype that you strive to emulate in your combat styles and techniques, such as Champion. The archetype you choose grants you features at 3rd level and again at 7th, 10th, 15th, and 18th level.</t>
   </si>
   <si>
@@ -171,9 +165,6 @@
     <t>Guardian Moves</t>
   </si>
   <si>
-    <t>You gain a number of Guardian Reactions equal to your proficiency bonus, and they recover on a short or long rest. You may use them for anything you could use a regular reaction for, or you can use them for special Guardian Moves. You can only use one Guardian Reaction a turn (but you may use a regular reaction and a Guardian Reaction in the same turn.)</t>
-  </si>
-  <si>
     <t>Guardian's have special reactive moves they can use to keep their allies safe. You must use a Guardian Reaction (not a regular reaction) to activate these moves.</t>
   </si>
   <si>
@@ -219,24 +210,10 @@
     <t>Ranger Spell Slots</t>
   </si>
   <si>
-    <t>The Ranger table shows how many spell slots you have to cast your spells of 1st level and higher. To cast one of these spells, you must expend a slot of the spell’s level or higher. You regain all expended spell slots when you finish a long rest.
-For example, if you know the 1st-level spell animal friendship and have a 1st-level and a 2nd-level spell slot available, you can cast animal friendship using either slot.</t>
-  </si>
-  <si>
     <t>Ranger Spells Known of 1st Level and Higher</t>
   </si>
   <si>
-    <t>You know two 1st-level spells of your choice from the ranger spell list.
-The Spells Known column of the Ranger table shows when you learn more ranger spells of your choice. Each of these spells must be of a level for which you have spell slots. For instance, when you reach 5th level in this class, you can learn one new spell of 1st or 2nd level.
-Additionally, when you gain a level in this class, you can choose one of the ranger spells you know and replace it with another spell from the ranger spell list, which also must be of a level for which you have spell slots.</t>
-  </si>
-  <si>
     <t>Ranger Spellcasting Ability</t>
-  </si>
-  <si>
-    <t>Wisdom is your spellcasting ability for your ranger spells, since your magic draws on your attunement to nature. You use your Wisdom whenever a spell refers to your spellcasting ability. In addition, you use your Wisdom modifier when setting the saving throw DC for a ranger spell you cast and when making an attack roll with one.
-Spell save DC = 8 + your proficiency bonus + your Wisdom modifier
-Spell attack modifier = your proficiency bonus + your Wisdom modifier</t>
   </si>
   <si>
     <t>Ranger Spellcasting Focus</t>
@@ -298,17 +275,9 @@
     <t>Spells of the Animal Whisperer</t>
   </si>
   <si>
-    <t>You learn the Find Familiar spell.
-You also learn the Animal Friendship and Speak with Animals spells if you do not already know them, or a new ranger spell for each one you do know.
-You can cast speak with animals at will, without expending a spell slot.</t>
-  </si>
-  <si>
     <t>Primeval Awareness</t>
   </si>
   <si>
-    <t>Beginning at 3rd level, you can use your action and expend one ranger spell slot to focus your awareness on the region around you. For 1 minute per level of the spell slot you expend, you can sense whether the following types of creatures are present within 1 mile of you (or within up to 6 miles if you are in your favored terrain): aberrations, celestials, dragons, elementals, fey, fiends, and undead. This feature doesn’t reveal the creatures’ location or number.</t>
-  </si>
-  <si>
     <t>Python script adds Primeval Awareness to features</t>
   </si>
   <si>
@@ -330,16 +299,9 @@
     <t>Monster Hunter Ranger</t>
   </si>
   <si>
-    <t>A Monster Hunter focuses on hunting down different creatures. The Monster Hunter philosophy understands that nature is often kill-or-be-killed; it is not wrong for a wolf to hunt down a new foal for food, nor is it wrong for a stag to kill the wolf to protect it's offspring. Monster Hunters believe in mastering their hunting skills in a kill-or-be-killed world.</t>
-  </si>
-  <si>
     <t>Aim for the Weak Spot</t>
   </si>
   <si>
-    <t>As a Bonus Action, a Monster Hunter may study a creature they have applied Hunter's Mark on. The next attack the Monster Hunter makes towards that creature is an automatic critical hit.
-A creature may only be the target of this once per day, and the Monster Hunter cannot use this ability again until they complete a short or long rest.</t>
-  </si>
-  <si>
     <t>Wizard Spellcasting</t>
   </si>
   <si>
@@ -355,25 +317,10 @@
     <t>Wizard Spellbook</t>
   </si>
   <si>
-    <t>At 1st level, you have a spellbook containing six 1st-­‐‑ level wizard spells of your choice. Your spellbook is the repository of the wizard spells you know, except your cantrips, which are fixed in your mind.</t>
-  </si>
-  <si>
     <t>Wizard Preparing and Casting Spells</t>
   </si>
   <si>
-    <t>The Wizard table shows how many spell slots you have to cast your spells of 1st level and higher. To cast one of these spells, you must expend a slot of the spell’s level or higher. You regain all expended spell slots when you finish a long rest.
-You prepare the list of wizard spells that are available for you to cast. To do so, choose a number of wizard spells from your spellbook equal to your Intelligence modifier + your wizard level (minimum of one spell). The spells must be of a level for which you have spell slots.
-For example, if you’re a 3rd-level wizard, you have four 1st-level and two 2nd-level spell slots. With an Intelligence of 16, your list of prepared spells can include six spells of 1st or 2nd level, in any combination, chosen from your spellbook. If you prepare the 1st-level spell magic missile, you can cast it using a 1st-level or a 2nd-level slot. Casting the spell doesn’t remove it from your list of prepared spells.
-You can change your list of prepared spells when you finish a long rest. Preparing a new list of wizard spells requires time spent studying your spellbook and memorizing the incantations and gestures you must make to cast the spell: at least 1 minute per spell level for each spell on your list.</t>
-  </si>
-  <si>
     <t>Wizard Spellcasting Ability</t>
-  </si>
-  <si>
-    <t>"Wisdom is your spellcasting ability for your ranger spells, since your magic draws on your attunement to nature. You use your Wisdom whenever a spell refers to your spellcasting ability. In addition, you use your Wisdom modifier when setting the saving throw DC for a ranger spell you cast and when making an attack roll with one.  Spell save DC = 8 + your proficiency bonus + your Wisdom modifier  Spell attack modifier = your proficiency bonus + your Wisdom modifier"
-Intelligence is your spellcasting ability for your wizard spells, since you learn your spells through dedicated study and memorization. You use your Intelligence whenever a spell refers to your spellcasting ability. In addition, you use your Intelligence modifier when setting the saving throw DC for a wizard spell you cast and when making an attack roll with one. 
-Spell save DC = 8 + your proficiency bonus + your Intelligence modifier
-Spell attack modifier = your proficiency bonus + your Intelligence modifier</t>
   </si>
   <si>
     <t>Wizard Ritual Casting</t>
@@ -426,17 +373,9 @@
     <t>Arcane Recovery</t>
   </si>
   <si>
-    <t>You have learned to regain some of your magical energy by studying your spellbook. Once per day when you finish a short rest, you can choose expended spell slots to recover. The spell slots can have a combined level that is equal to or less than half your wizard level (rounded up), and none of the slots can be 6th level or higher.
-For example, if you’re a 4th-level wizard, you can recover up to two levels worth of spell slots. You can recover either a 2nd-level spell slot or two 1st-level spell slots.</t>
-  </si>
-  <si>
     <t>Arcane Tradition</t>
   </si>
   <si>
-    <t>When you reach 2nd level, you choose an arcane tradition, shaping your practice of magic.
-Your choice grants you features at 2nd level and again at 6th, 10th, and 14th level.</t>
-  </si>
-  <si>
     <t>Tradition of Destruction</t>
   </si>
   <si>
@@ -446,9 +385,6 @@
     <t>Sculpt Spells</t>
   </si>
   <si>
-    <t>Beginning at 2nd level, you can create pockets of relative safety within the effects of your evocation spells. When you cast an evocation spell that affects other creatures that you can see, you can choose a number of them equal to 1 + the spell’s level. The chosen creatures automatically succeed on their saving throws against the spell, and they take no damage if they would normally take half damage on a successful save.</t>
-  </si>
-  <si>
     <t>Tradition of Chronomancy</t>
   </si>
   <si>
@@ -456,9 +392,6 @@
   </si>
   <si>
     <t>Branching Fate</t>
-  </si>
-  <si>
-    <t>You magically alter the flow of time around you. As a reaction, after you or a creature you can see within 30 feet of you makes an attack roll, an ability check, or a saving throw, you can force the creature to reroll. You make this decision after you see whether the roll succeeds or fails. You can then choose whether the target uses the result of the first or second roll. You can't use this ability again until you complete a short or long rest.You magically alter the flow of time around you. As a reaction, after you or a creature you can see within 30 feet of you makes an attack roll, an ability check, or a saving throw, you can force the creature to reroll. You make this decision after you see whether the roll succeeds or fails. You can then choose whether the target uses the result of the first or second roll.</t>
   </si>
   <si>
     <t>Python Script offers choice of Arcane Tradition, then adds corresponding ability (or abilities) of the tradition.</t>
@@ -472,7 +405,133 @@
 add two spells of the highest level wizard spell we can cast to spellbook (3rd level spells now)</t>
   </si>
   <si>
-    <t>pc_feature_description</t>
+    <t>At 1st level, you have a spellbook containing six 1st  level wizard spells of your choice. Your spellbook is the repository of the wizard spells you know, except your cantrips, which are fixed in your mind.</t>
+  </si>
+  <si>
+    <t>When you roll a 1 or 2 on a damage die for an attack you make with a two-handed melee weapon (or a versatile melee weaponthat you are wielding with two hands), you can reroll the die and must use the new roll, even if the new roll is a 1 or a 2.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Once you use this feature, you must finish a short or long rest before you can use it again. Starting at 17th level, you can use it twice before a rest, but only once on the same turn. </t>
+  </si>
+  <si>
+    <t>pc_feature_description_line_1</t>
+  </si>
+  <si>
+    <t>pc_feature_description_line_2</t>
+  </si>
+  <si>
+    <t>Starting at 2nd level Fighter, you can push yourself beyond your normal limits for a moment. On your turn, you can take one additional action on top of your regular action and a possible bonus action.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You gain a number of Guardian Reactions equal to your proficiency bonus, and they recover on a short or long rest. You may use them for anything you could use a regular reaction for, or you can use them for special Guardian Moves. </t>
+  </si>
+  <si>
+    <t>You can only use one Guardian Reaction a turn (but you may use a regular reaction and a Guardian Reaction in the same turn.)</t>
+  </si>
+  <si>
+    <t>The Ranger table shows how many spell slots you have to cast your spells of 1st level and higher. To cast one of these spells, you must expend a slot of the spell’s level or higher. You regain all expended spell slots when you finish a long rest.</t>
+  </si>
+  <si>
+    <t>For example, if you know the 1st-level spell animal friendship and have a 1st-level and a 2nd-level spell slot available, you can cast animal friendship using either slot.</t>
+  </si>
+  <si>
+    <t>pc_feature_description_line_3</t>
+  </si>
+  <si>
+    <t>You know two 1st-level spells of your choice from the ranger spell list.</t>
+  </si>
+  <si>
+    <t>The Spells Known column of the Ranger table shows when you learn more ranger spells of your choice. Each of these spells must be of a level for which you have spell slots. For instance, when you reach 5th level in this class, you can learn one new spell of 1st or 2nd level.</t>
+  </si>
+  <si>
+    <t>Additionally, when you gain a level in this class, you can choose one of the ranger spells you know and replace it with another spell from the ranger spell list, which also must be of a level for which you have spell slots.</t>
+  </si>
+  <si>
+    <t>For 1 minute per level of the spell slot you expend, you can sense whether the following types of creatures are present within 6 miles of you: aberrations, celestials, dragons, elementals, fey, fiends, and undead. This feature doesn’t reveal the creatures’ location or number.</t>
+  </si>
+  <si>
+    <t>A Monster Hunter Ranger focuses on being the best possible hunter they can be. In the kill-or-be-killed world of nature, where predators hunt to survive and prey fight off hunters to survive, only the strongest lives. The Monster Hunter seeks to be the strongest.</t>
+  </si>
+  <si>
+    <t>As a Bonus Action, a Monster Hunter may study a creature they have applied Hunter's Mark on. The next attack the Monster Hunter makes towards that creature is an automatic critical hit.</t>
+  </si>
+  <si>
+    <t>A creature may only be the target of this once per day, and the Monster Hunter cannot use this ability again until they complete a short or long rest.</t>
+  </si>
+  <si>
+    <t>You also learn the Animal Friendship and Speak with Animals spells if you do not already know them, or a new ranger spell for each one you do know.</t>
+  </si>
+  <si>
+    <t>You can cast speak with animals at will, without expending a spell slot.</t>
+  </si>
+  <si>
+    <t>You learn the Find Familiar spell.</t>
+  </si>
+  <si>
+    <t>pc_feature_description_line_4</t>
+  </si>
+  <si>
+    <t>You prepare the list of wizard spells that are available for you to cast. To do so, choose a number of wizard spells from your spellbook equal to your Intelligence modifier + your wizard level (minimum of one spell). The spells must be of a level for which you have spell slots.</t>
+  </si>
+  <si>
+    <t>For example, if you’re a 3rd-level wizard, you have four 1st-level and two 2nd-level spell slots. With an Intelligence of 16, your list of prepared spells can include six spells of 1st or 2nd level, in any combination, chosen from your spellbook. If you prepare the 1st-level spell magic missile, you can cast it using a 1st-level or a 2nd-level slot. Casting the spell doesn’t remove it from your list of prepared spells.</t>
+  </si>
+  <si>
+    <t>You can change your list of prepared spells when you finish a long rest. Preparing a new list of wizard spells requires time spent studying your spellbook and memorizing the incantations and gestures you must make to cast the spell: at least 1 minute per spell level for each spell on your list.</t>
+  </si>
+  <si>
+    <t>The Wizard table shows how many spell slots you have to cast your spells of 1st level and higher. To cast one of these spells, you must expend a slot of the spell’s level or higher. You regain all expended spell slots when you finish a long rest.</t>
+  </si>
+  <si>
+    <t>Beginning at 3rd level, you can use your action and expend one ranger spell slot to focus your awareness on the region around you.</t>
+  </si>
+  <si>
+    <t>For example, if you’re a 4th-level wizard, you can recover up to two levels worth of spell slots. You can recover either a 2nd-level spell slot or two 1st-level spell slots.</t>
+  </si>
+  <si>
+    <t>When you reach 2nd level, you choose an arcane tradition, shaping your practice of magic.</t>
+  </si>
+  <si>
+    <t>Your choice grants you features at 2nd level and again at 6th, 10th, and 14th level.</t>
+  </si>
+  <si>
+    <t>Beginning at 2nd level, you can create pockets of relative safety within the effects of your evocation spells.</t>
+  </si>
+  <si>
+    <t>When you cast an evocation spell that affects other creatures that you can see, you can choose a number of them equal to 1 + the spell’s level. The chosen creatures automatically succeed on their saving throws against the spell, and they take no damage if they would normally take half damage on a successful save.</t>
+  </si>
+  <si>
+    <t>After using this ability, you can't use it again until you complete a short or long rest.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You magically alter the flow of time around you. As a reaction, after you or a creature you can see within 30 feet of you makes an attack roll, an ability check, or a saving throw, you can force the creature to roll again. </t>
+  </si>
+  <si>
+    <t>You may make this decision after you see whether the roll succeeds or fails. You can then choose whether the target uses the result of the first or second roll.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You have learned to regain some of your magical energy by studying your spellbook. </t>
+  </si>
+  <si>
+    <t>Once per day when you finish a short rest, you can choose expended spell slots to recover. The spell slots can have a combined level that is equal to or less than half your wizard level (rounded up), and none of the slots can be 6th level or higher.</t>
+  </si>
+  <si>
+    <t>Intelligence is your spellcasting ability for your wizard spells, since you learn your spells through dedicated study and memorization. You use your Intelligence whenever a spell refers to your spellcasting ability.</t>
+  </si>
+  <si>
+    <t>You use your Intelligence modifier when setting the Spell Save DC for a wizard spell you cast;  Spell Save DC = 8 + your proficiency bonus + your Intelligence modifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You also use your Intelligence modifier when making an attack roll with a Spell:  Spell attack modifier = your proficiency bonus + your Intelligence modifier </t>
+  </si>
+  <si>
+    <t>Wisdom is your spellcasting ability for your ranger spells, since your magic draws on your attunement to nature. You use your Wisdom whenever a spell refers to your spellcasting ability.</t>
+  </si>
+  <si>
+    <t>You use your Wisdom modifier when setting the Spell Save DC for a ranger spell you cast; Spell save DC = 8 + your proficiency bonus + your Wisdom modifier</t>
+  </si>
+  <si>
+    <t>You also use your Wisdom modifier when making an attack roll with a Spell: Spell attack modifier = your proficiency bonus + your Wisdom modifier</t>
   </si>
 </sst>
 </file>
@@ -540,7 +599,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -561,6 +620,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -875,21 +938,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94DF8C6D-E654-4DC1-9038-77E4A221C97E}">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="99.5703125" customWidth="1"/>
+    <col min="4" max="4" width="255.42578125" customWidth="1"/>
+    <col min="5" max="5" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="209.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -897,13 +960,22 @@
         <v>21</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="E1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -917,7 +989,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -931,7 +1003,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -945,7 +1017,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -959,7 +1031,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -970,10 +1042,10 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -987,7 +1059,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1001,7 +1073,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1015,21 +1087,24 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="9">
+        <v>0</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1040,10 +1115,10 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1054,10 +1129,10 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1068,488 +1143,551 @@
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="E19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C26">
         <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="E27" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C28">
         <v>1</v>
       </c>
-      <c r="D28" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="E28" t="s">
+        <v>128</v>
+      </c>
+      <c r="F28" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C29">
         <v>1</v>
       </c>
-      <c r="D29" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="F29" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C30">
         <v>0</v>
       </c>
-      <c r="D30" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D30" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="E30" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C31">
         <v>0</v>
       </c>
       <c r="D31" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C32">
         <v>1</v>
       </c>
-      <c r="D32" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D32" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E32" t="s">
+        <v>134</v>
+      </c>
+      <c r="F32" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C33">
         <v>0</v>
       </c>
       <c r="D33" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C34">
         <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+      <c r="E34" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="C35">
         <v>0</v>
       </c>
       <c r="D35" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C36">
         <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C37">
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="C38">
         <v>1</v>
       </c>
-      <c r="D38" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="E38" t="s">
+        <v>138</v>
+      </c>
+      <c r="F38" t="s">
+        <v>139</v>
+      </c>
+      <c r="G38" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="C39">
         <v>1</v>
       </c>
-      <c r="D39" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="E39" t="s">
+        <v>154</v>
+      </c>
+      <c r="F39" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="C40">
         <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="C41">
         <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="C42">
         <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="C43">
         <v>0</v>
       </c>
-      <c r="D43" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D43" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="E43" t="s">
+        <v>152</v>
+      </c>
+      <c r="F43" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="C44">
         <v>0</v>
       </c>
-      <c r="D44" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D44" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E44" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="C45">
         <v>0</v>
       </c>
       <c r="D45" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C46">
         <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+      <c r="E46" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="C47">
         <v>0</v>
       </c>
       <c r="D47" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="C48">
         <v>1</v>
       </c>
-      <c r="D48" t="s">
-        <v>129</v>
+      <c r="D48" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="E48" t="s">
+        <v>150</v>
+      </c>
+      <c r="F48" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -1574,10 +1712,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1588,7 +1726,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1599,7 +1737,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1610,7 +1748,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1621,7 +1759,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1632,7 +1770,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1643,17 +1781,17 @@
         <v>0</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C9" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C12" s="5" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1661,10 +1799,10 @@
         <v>1</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1672,10 +1810,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1683,10 +1821,10 @@
         <v>1</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1694,10 +1832,10 @@
         <v>2</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1705,10 +1843,10 @@
         <v>2</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1716,10 +1854,10 @@
         <v>2</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1727,10 +1865,10 @@
         <v>3</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1738,10 +1876,10 @@
         <v>3</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1749,10 +1887,10 @@
         <v>3</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1760,10 +1898,10 @@
         <v>3</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1771,10 +1909,10 @@
         <v>4</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1782,10 +1920,10 @@
         <v>4</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1793,10 +1931,10 @@
         <v>5</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1804,10 +1942,10 @@
         <v>5</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1815,10 +1953,10 @@
         <v>5</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -1826,10 +1964,10 @@
         <v>1</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1837,10 +1975,10 @@
         <v>1</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1848,10 +1986,10 @@
         <v>1</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1859,10 +1997,10 @@
         <v>1</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1870,10 +2008,10 @@
         <v>2</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1881,10 +2019,10 @@
         <v>2</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1892,10 +2030,10 @@
         <v>3</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1903,10 +2041,10 @@
         <v>4</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1914,10 +2052,10 @@
         <v>4</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1925,10 +2063,10 @@
         <v>5</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created character features, exported to CSV, added database import
</commit_message>
<xml_diff>
--- a/Main/static/CSVs/PC Features List.xlsx
+++ b/Main/static/CSVs/PC Features List.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitProjects\CS50-FinalProject\Main\static\CSVs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52153E2-E89D-4677-B484-2A6C5E86BB66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70B72B0-0BA9-499F-98D1-27044B0D71C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B488902C-D55E-47C3-8D97-FFB9C3833CE3}"/>
   </bookViews>
   <sheets>
-    <sheet name="pc_feature_list" sheetId="4" r:id="rId1"/>
-    <sheet name="PC_level_up pseudo-code" sheetId="6" r:id="rId2"/>
-    <sheet name="individual_pc_features" sheetId="5" r:id="rId3"/>
+    <sheet name="pc_features_list" sheetId="4" r:id="rId1"/>
+    <sheet name="character_level_up pseudo-code" sheetId="6" r:id="rId2"/>
+    <sheet name="individual_character_features" sheetId="5" r:id="rId3"/>
     <sheet name="Metadata" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -599,7 +599,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -623,7 +623,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -938,9 +937,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94DF8C6D-E654-4DC1-9038-77E4A221C97E}">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1087,20 +1088,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10">
         <v>0</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1303,23 +1304,35 @@
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>58</v>
+        <v>124</v>
+      </c>
+      <c r="E26" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1327,16 +1340,19 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
-      <c r="D27" t="s">
-        <v>124</v>
+      <c r="D27" s="8" t="s">
+        <v>127</v>
       </c>
       <c r="E27" t="s">
-        <v>125</v>
+        <v>128</v>
+      </c>
+      <c r="F27" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1344,19 +1360,19 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C28">
         <v>1</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="E28" t="s">
-        <v>128</v>
+        <v>156</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>157</v>
       </c>
       <c r="F28" t="s">
-        <v>129</v>
+        <v>158</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1364,19 +1380,16 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="F29" t="s">
-        <v>158</v>
+        <v>142</v>
+      </c>
+      <c r="E29" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1384,16 +1397,13 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C30">
         <v>0</v>
       </c>
-      <c r="D30" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="E30" t="s">
-        <v>130</v>
+      <c r="D30" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1401,13 +1411,19 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C31">
-        <v>0</v>
-      </c>
-      <c r="D31" t="s">
-        <v>72</v>
+        <v>1</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E31" t="s">
+        <v>134</v>
+      </c>
+      <c r="F31" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1415,19 +1431,13 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="C32">
-        <v>1</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="E32" t="s">
-        <v>134</v>
-      </c>
-      <c r="F32" t="s">
-        <v>135</v>
+        <v>0</v>
+      </c>
+      <c r="D32" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1435,13 +1445,16 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>131</v>
+        <v>132</v>
+      </c>
+      <c r="E33" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1449,16 +1462,13 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D34" t="s">
-        <v>132</v>
-      </c>
-      <c r="E34" t="s">
-        <v>133</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1466,13 +1476,13 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1480,13 +1490,13 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C36">
         <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1494,13 +1504,22 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C37">
         <v>1</v>
       </c>
-      <c r="D37" t="s">
-        <v>116</v>
+      <c r="D37" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="E37" t="s">
+        <v>138</v>
+      </c>
+      <c r="F37" t="s">
+        <v>139</v>
+      </c>
+      <c r="G37" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1508,22 +1527,19 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C38">
         <v>1</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="E38" t="s">
-        <v>138</v>
+        <v>154</v>
       </c>
       <c r="F38" t="s">
-        <v>139</v>
-      </c>
-      <c r="G38" t="s">
-        <v>140</v>
+        <v>155</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -1531,19 +1547,13 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C39">
         <v>1</v>
       </c>
-      <c r="D39" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="E39" t="s">
-        <v>154</v>
-      </c>
-      <c r="F39" t="s">
-        <v>155</v>
+      <c r="D39" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -1551,13 +1561,13 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C40">
         <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -1565,13 +1575,13 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C41">
         <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -1579,13 +1589,19 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="C42">
-        <v>1</v>
-      </c>
-      <c r="D42" t="s">
-        <v>95</v>
+        <v>0</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="E42" t="s">
+        <v>152</v>
+      </c>
+      <c r="F42" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -1593,19 +1609,16 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C43">
         <v>0</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="E43" t="s">
-        <v>152</v>
-      </c>
-      <c r="F43" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -1613,16 +1626,13 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C44">
         <v>0</v>
       </c>
-      <c r="D44" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="E44" t="s">
-        <v>145</v>
+      <c r="D44" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -1630,13 +1640,16 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D45" t="s">
-        <v>108</v>
+        <v>146</v>
+      </c>
+      <c r="E45" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -1644,16 +1657,13 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D46" t="s">
-        <v>146</v>
-      </c>
-      <c r="E46" t="s">
-        <v>147</v>
+        <v>111</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -1661,32 +1671,18 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C47">
-        <v>0</v>
-      </c>
-      <c r="D47" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>46</v>
-      </c>
-      <c r="B48" t="s">
-        <v>112</v>
-      </c>
-      <c r="C48">
-        <v>1</v>
-      </c>
-      <c r="D48" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D47" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E47" t="s">
         <v>150</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F47" t="s">
         <v>148</v>
       </c>
     </row>
@@ -1700,7 +1696,7 @@
   <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2080,7 +2076,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2105,6 +2101,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>